<commit_message>
Added var usage tree, need to actually evaluate it at the end.
</commit_message>
<xml_diff>
--- a/SplCompiler/Todo.xlsx
+++ b/SplCompiler/Todo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\LanguagesAndCompilers\SplCompiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66C5076A-5B87-4F46-BDBC-A368AD636033}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BBC239-5551-41E3-B832-EE22FF3A9D02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{50EF48C9-6323-418F-8AB0-BA98C6E84C2C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
   <si>
     <t>Test</t>
   </si>
@@ -161,9 +161,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Should have ability to test for runtime errors too, e.g. does compiler prevent constant divide by zero or  etc? Maybe type=rterror?</t>
-  </si>
-  <si>
     <t>invalid char input</t>
   </si>
   <si>
@@ -189,6 +186,12 @@
   </si>
   <si>
     <t>Needs reworking</t>
+  </si>
+  <si>
+    <t>Me</t>
+  </si>
+  <si>
+    <t>Length of var name checks</t>
   </si>
 </sst>
 </file>
@@ -224,13 +227,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075A21D6-570E-47A5-875C-908BD7B48656}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,7 +573,7 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -590,7 +590,7 @@
         <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -607,7 +607,7 @@
         <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -646,7 +646,7 @@
         <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -660,10 +660,10 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
         <v>51</v>
-      </c>
-      <c r="E7" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -800,40 +800,41 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
         <v>45</v>
       </c>
-      <c r="B20" t="s">
-        <v>46</v>
-      </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
         <v>45</v>
       </c>
-      <c r="B21" t="s">
-        <v>46</v>
-      </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A23:C23"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Still passing all tests. Variable warnings and errors working. Constant value checks are working (real and integer limits).
</commit_message>
<xml_diff>
--- a/SplCompiler/Todo.xlsx
+++ b/SplCompiler/Todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\LanguagesAndCompilers\SplCompiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BBC239-5551-41E3-B832-EE22FF3A9D02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEF435B-9F2D-4F7E-A8EE-0063C15A96C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{50EF48C9-6323-418F-8AB0-BA98C6E84C2C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
   <si>
     <t>Test</t>
   </si>
@@ -182,16 +182,22 @@
     <t xml:space="preserve"> does compiler prevent constant divide by zero</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Needs reworking</t>
-  </si>
-  <si>
     <t>Me</t>
   </si>
   <si>
     <t>Length of var name checks</t>
+  </si>
+  <si>
+    <t>Reworked with a tree for variable usages.</t>
+  </si>
+  <si>
+    <t>Tests pass</t>
+  </si>
+  <si>
+    <t>Sets value to INT_MAX</t>
+  </si>
+  <si>
+    <t>Sets value to INT_MIN</t>
   </si>
 </sst>
 </file>
@@ -230,7 +236,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,7 +554,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,10 +666,10 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -709,6 +715,9 @@
       <c r="C11" t="s">
         <v>25</v>
       </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -720,6 +729,9 @@
       <c r="C12" t="s">
         <v>26</v>
       </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -731,6 +743,12 @@
       <c r="C13" t="s">
         <v>29</v>
       </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -742,6 +760,12 @@
       <c r="C14" t="s">
         <v>31</v>
       </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -765,7 +789,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
@@ -776,7 +800,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
@@ -786,8 +810,14 @@
       <c r="C18" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
@@ -797,8 +827,14 @@
       <c r="C19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
@@ -809,7 +845,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
@@ -823,15 +859,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added assignment checks for type conversions
</commit_message>
<xml_diff>
--- a/SplCompiler/Todo.xlsx
+++ b/SplCompiler/Todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\LanguagesAndCompilers\SplCompiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEF435B-9F2D-4F7E-A8EE-0063C15A96C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0D69E3-DBCA-4042-8AE0-3D66BA13F8E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{50EF48C9-6323-418F-8AB0-BA98C6E84C2C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
   <si>
     <t>Test</t>
   </si>
@@ -179,9 +179,6 @@
     <t>Name mangling allows this</t>
   </si>
   <si>
-    <t xml:space="preserve"> does compiler prevent constant divide by zero</t>
-  </si>
-  <si>
     <t>Me</t>
   </si>
   <si>
@@ -198,6 +195,33 @@
   </si>
   <si>
     <t>Sets value to INT_MIN</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Warning generated</t>
+  </si>
+  <si>
+    <t>Warning generated warns loss of precision</t>
+  </si>
+  <si>
+    <t>Constant folding</t>
+  </si>
+  <si>
+    <t>Loop unwinding</t>
+  </si>
+  <si>
+    <t>Redundant assignment removal</t>
+  </si>
+  <si>
+    <t>does compiler prevent constant divide by zero</t>
+  </si>
+  <si>
+    <t>Yes removes all until read a valid string. Removes white space. Flushes after reading.</t>
+  </si>
+  <si>
+    <t>All variables are initilised to one.</t>
   </si>
 </sst>
 </file>
@@ -551,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075A21D6-570E-47A5-875C-908BD7B48656}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,7 +586,7 @@
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="3" max="3" width="123" customWidth="1"/>
     <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -669,7 +693,7 @@
         <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -682,6 +706,12 @@
       <c r="C8" t="s">
         <v>19</v>
       </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -693,6 +723,12 @@
       <c r="C9" t="s">
         <v>20</v>
       </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -704,6 +740,9 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -747,7 +786,7 @@
         <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -764,7 +803,7 @@
         <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -777,6 +816,12 @@
       <c r="C15" t="s">
         <v>32</v>
       </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -799,6 +844,12 @@
       <c r="C17" t="s">
         <v>36</v>
       </c>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
@@ -814,7 +865,7 @@
         <v>42</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -831,7 +882,7 @@
         <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -842,7 +893,7 @@
         <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -858,16 +909,52 @@
       <c r="D21" t="s">
         <v>42</v>
       </c>
+      <c r="E21" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
         <v>50</v>
       </c>
-      <c r="C22" t="s">
-        <v>51</v>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added warnings to generated code when it clears chars from the stdin. Wrote a simple calculator in SPL
</commit_message>
<xml_diff>
--- a/SplCompiler/Todo.xlsx
+++ b/SplCompiler/Todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\LanguagesAndCompilers\SplCompiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FAAA3E7-7C61-4220-BA5B-773310BB6E01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558C4AF5-7B7E-41E4-9600-5AD26580E698}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{50EF48C9-6323-418F-8AB0-BA98C6E84C2C}"/>
+    <workbookView xWindow="-21710" yWindow="-16870" windowWidth="21820" windowHeight="38020" xr2:uid="{50EF48C9-6323-418F-8AB0-BA98C6E84C2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="67">
   <si>
     <t>Test</t>
   </si>
@@ -209,9 +209,6 @@
     <t>Constant folding</t>
   </si>
   <si>
-    <t>Loop unwinding</t>
-  </si>
-  <si>
     <t>Redundant assignment removal</t>
   </si>
   <si>
@@ -230,7 +227,10 @@
     <t>Constant folding should be done</t>
   </si>
   <si>
-    <t>Swap constant identifiers</t>
+    <t>Fix do while shift reduce if change statement_list to code</t>
+  </si>
+  <si>
+    <t>Remves and warns</t>
   </si>
 </sst>
 </file>
@@ -246,12 +246,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -266,10 +272,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075A21D6-570E-47A5-875C-908BD7B48656}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -616,36 +624,36 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -672,164 +680,167 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
-        <v>42</v>
-      </c>
+      <c r="D10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D11" t="s">
-        <v>42</v>
-      </c>
+      <c r="D11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D12" t="s">
-        <v>42</v>
-      </c>
+      <c r="D12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" t="s">
-        <v>63</v>
+      <c r="D15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -844,53 +855,53 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="D19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>52</v>
       </c>
     </row>
@@ -902,24 +913,24 @@
         <v>45</v>
       </c>
       <c r="C20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -934,31 +945,37 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D23" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" t="s">
-        <v>65</v>
+      <c r="D23" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="3" t="s">
         <v>59</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -969,7 +986,7 @@
         <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -980,18 +997,7 @@
         <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented checks to prevent the multipulcation and division of chars
</commit_message>
<xml_diff>
--- a/SplCompiler/Todo.xlsx
+++ b/SplCompiler/Todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\LanguagesAndCompilers\SplCompiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558C4AF5-7B7E-41E4-9600-5AD26580E698}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B889D71D-438F-4C30-AA89-7295A1CABEBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21710" yWindow="-16870" windowWidth="21820" windowHeight="38020" xr2:uid="{50EF48C9-6323-418F-8AB0-BA98C6E84C2C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{50EF48C9-6323-418F-8AB0-BA98C6E84C2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="70">
   <si>
     <t>Test</t>
   </si>
@@ -231,6 +231,15 @@
   </si>
   <si>
     <t>Remves and warns</t>
+  </si>
+  <si>
+    <t>Cast will remove negative so is valid even if stupid…</t>
+  </si>
+  <si>
+    <t>Rejects.</t>
+  </si>
+  <si>
+    <t>Error</t>
   </si>
 </sst>
 </file>
@@ -275,9 +284,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075A21D6-570E-47A5-875C-908BD7B48656}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -624,284 +633,302 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="3"/>
+      <c r="D10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="3"/>
+      <c r="D11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="3"/>
+      <c r="D12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="D13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="D14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="D15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="B16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="D16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="B17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="D17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="3" t="s">
+      <c r="D18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="D19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>52</v>
       </c>
     </row>
@@ -917,19 +944,19 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="3" t="s">
+      <c r="D21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>61</v>
       </c>
     </row>
@@ -945,36 +972,36 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="D23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="D24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added extra tests to operators.spl
</commit_message>
<xml_diff>
--- a/SplCompiler/Todo.xlsx
+++ b/SplCompiler/Todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\LanguagesAndCompilers\SplCompiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B889D71D-438F-4C30-AA89-7295A1CABEBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81B55FE-3612-46BA-9BC9-D57AFEDFCE36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{50EF48C9-6323-418F-8AB0-BA98C6E84C2C}"/>
   </bookViews>
@@ -604,7 +604,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Implemented static division by zero checks
</commit_message>
<xml_diff>
--- a/SplCompiler/Todo.xlsx
+++ b/SplCompiler/Todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\LanguagesAndCompilers\SplCompiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81B55FE-3612-46BA-9BC9-D57AFEDFCE36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCF48B1-4E4E-4D69-AF33-B61D35164B72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{50EF48C9-6323-418F-8AB0-BA98C6E84C2C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
   <si>
     <t>Test</t>
   </si>
@@ -240,6 +240,12 @@
   </si>
   <si>
     <t>Error</t>
+  </si>
+  <si>
+    <t>Dead code</t>
+  </si>
+  <si>
+    <t>Loop Unrolling</t>
   </si>
 </sst>
 </file>
@@ -601,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075A21D6-570E-47A5-875C-908BD7B48656}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1027,6 +1033,34 @@
         <v>65</v>
       </c>
     </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added identifier length check
</commit_message>
<xml_diff>
--- a/SplCompiler/Todo.xlsx
+++ b/SplCompiler/Todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\LanguagesAndCompilers\SplCompiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCF48B1-4E4E-4D69-AF33-B61D35164B72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC1047C-6F7F-4C8F-B28B-3683BDC60120}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{50EF48C9-6323-418F-8AB0-BA98C6E84C2C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="73">
   <si>
     <t>Test</t>
   </si>
@@ -209,9 +209,6 @@
     <t>Constant folding</t>
   </si>
   <si>
-    <t>Redundant assignment removal</t>
-  </si>
-  <si>
     <t>does compiler prevent constant divide by zero</t>
   </si>
   <si>
@@ -242,10 +239,16 @@
     <t>Error</t>
   </si>
   <si>
-    <t>Dead code</t>
-  </si>
-  <si>
     <t>Loop Unrolling</t>
+  </si>
+  <si>
+    <t>Dead store</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Static</t>
   </si>
 </sst>
 </file>
@@ -287,12 +290,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075A21D6-570E-47A5-875C-908BD7B48656}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,7 +690,7 @@
         <v>55</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -703,7 +707,7 @@
         <v>42</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -867,7 +871,7 @@
         <v>42</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -884,7 +888,7 @@
         <v>42</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -946,7 +950,13 @@
         <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -963,7 +973,7 @@
         <v>42</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -991,24 +1001,18 @@
         <v>42</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>66</v>
+      <c r="C24" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1019,17 +1023,23 @@
         <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1041,24 +1051,7 @@
         <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" t="s">
-        <v>71</v>
-      </c>
-      <c r="D28" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>